<commit_message>
update and add admin files
</commit_message>
<xml_diff>
--- a/Admin/Program_Map.xlsx
+++ b/Admin/Program_Map.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_550\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khunter/Dropbox/mordred/Power-Under-Multiplicity/Admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2D87D81-4DD4-4C38-8468-E32B386D9AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C15F4B-6241-7146-AA89-858C37DD9C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="12405" windowHeight="14370" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28200" yWindow="860" windowWidth="25320" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="fromthepaper" sheetId="1" r:id="rId1"/>
-    <sheet name="Files and Programs" sheetId="3" r:id="rId2"/>
-    <sheet name="Data File Naming Convention" sheetId="5" r:id="rId3"/>
-    <sheet name="File map new" sheetId="7" r:id="rId4"/>
-    <sheet name="File map old" sheetId="6" r:id="rId5"/>
+    <sheet name="Data File Naming Convention" sheetId="9" r:id="rId1"/>
+    <sheet name="fromthepaper" sheetId="1" r:id="rId2"/>
+    <sheet name="Files and Programs" sheetId="3" r:id="rId3"/>
+    <sheet name="Data File Naming Convention old" sheetId="5" r:id="rId4"/>
+    <sheet name="File map new" sheetId="7" r:id="rId5"/>
+    <sheet name="File map old" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="312">
   <si>
     <t>program name</t>
   </si>
@@ -1026,7 +1027,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,7 +1170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1219,12 +1220,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1314,6 +1352,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1338,11 +1382,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1697,6 +1759,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EE9C98-2FD9-0E46-A586-698033A2F0AD}">
+  <dimension ref="A5:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="60"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="12">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="60"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="12">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="12">
+        <v>2</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="12">
+        <v>2</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="12">
+        <v>3</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="12">
+        <v>3</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="12">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="12">
+        <v>2</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="12">
+        <v>3</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A12:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
@@ -1704,17 +2066,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +2096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1745,7 +2107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75">
+    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1759,7 +2121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1773,7 +2135,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1784,7 +2146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90">
+    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1795,7 +2157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105">
+    <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1809,7 +2171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1829,7 +2191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +2211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +2231,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1889,7 +2251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60">
+    <row r="12" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1909,7 +2271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1926,7 +2288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60">
+    <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1946,7 +2308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1963,7 +2325,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45">
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1980,7 +2342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +2359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45">
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2014,7 +2376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2031,7 +2393,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90">
+    <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2048,7 +2410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60">
+    <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2065,7 +2427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60">
+    <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2085,7 +2447,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60">
+    <row r="23" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2105,7 +2467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60">
+    <row r="24" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2122,7 +2484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="60">
+    <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -2139,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60">
+    <row r="26" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2159,7 +2521,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60">
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2176,7 +2538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="60">
+    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2193,7 +2555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="60">
+    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2210,7 +2572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="60">
+    <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2230,7 +2592,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2247,7 +2609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2264,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="60">
+    <row r="33" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -2278,7 +2640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -2292,7 +2654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="60">
+    <row r="35" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2312,7 +2674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
@@ -2320,21 +2682,21 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="67.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="12.75">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>58</v>
       </c>
@@ -2360,7 +2722,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="12.75">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>66</v>
       </c>
@@ -2373,7 +2735,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="51">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="8" t="s">
         <v>67</v>
@@ -2400,7 +2762,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" ht="38.25">
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
@@ -2424,7 +2786,7 @@
       </c>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" ht="25.5">
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
@@ -2450,7 +2812,7 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="63" customHeight="1">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
@@ -2476,7 +2838,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="51">
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
@@ -2502,7 +2864,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="38.25">
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
@@ -2528,7 +2890,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="25.5">
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
@@ -2554,7 +2916,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="61.5" customHeight="1">
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3" t="s">
@@ -2580,7 +2942,7 @@
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="87" customHeight="1">
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
@@ -2606,7 +2968,7 @@
       </c>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="27" customHeight="1">
+    <row r="12" spans="1:10" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3" t="s">
@@ -2632,7 +2994,7 @@
       </c>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" ht="12.75">
+    <row r="13" spans="1:10" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
@@ -2641,7 +3003,7 @@
       <c r="F13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" s="3" customFormat="1">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>110</v>
       </c>
@@ -2649,7 +3011,7 @@
       <c r="E14" s="7"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10" s="3" customFormat="1" ht="38.25">
+    <row r="15" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>111</v>
       </c>
@@ -2673,7 +3035,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="38.25">
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
         <v>115</v>
       </c>
@@ -2697,7 +3059,7 @@
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="36.75" customHeight="1">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="3" t="s">
         <v>119</v>
       </c>
@@ -2721,7 +3083,7 @@
       </c>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" ht="38.25">
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="C18" s="3" t="s">
         <v>123</v>
       </c>
@@ -2745,7 +3107,7 @@
       </c>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" s="3" customFormat="1" ht="37.5" customHeight="1">
+    <row r="19" spans="1:10" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="3" t="s">
         <v>125</v>
       </c>
@@ -2769,7 +3131,7 @@
       </c>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="26.25" customHeight="1">
+    <row r="20" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>127</v>
@@ -2794,7 +3156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.5">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
@@ -2819,16 +3181,16 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>132</v>
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>133</v>
@@ -2838,15 +3200,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
         <v>136</v>
@@ -2855,7 +3217,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>137</v>
@@ -2864,17 +3226,17 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
         <v>139</v>
@@ -2883,16 +3245,16 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="3" customFormat="1">
+    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>141</v>
       </c>
@@ -2909,7 +3271,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1">
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>145</v>
       </c>
@@ -2937,27 +3299,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE31590-FD64-45DE-80C6-3D53A6E7FB43}">
   <dimension ref="A5:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:10" ht="60">
+    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>147</v>
       </c>
@@ -2976,25 +3338,25 @@
       <c r="F5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="43" t="s">
         <v>153</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>155</v>
       </c>
@@ -3013,15 +3375,15 @@
       <c r="F7" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="44" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="45" t="s">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="45" t="s">
         <v>161</v>
       </c>
       <c r="C8" s="12">
@@ -3036,13 +3398,13 @@
       <c r="F8" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="G8" s="44" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="45"/>
-      <c r="B9" s="43"/>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="47"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="12">
         <v>2</v>
       </c>
@@ -3055,13 +3417,13 @@
       <c r="F9" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="44" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="45"/>
-      <c r="B10" s="43"/>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="47"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="12">
         <v>2</v>
       </c>
@@ -3074,13 +3436,13 @@
       <c r="F10" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="44" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="45"/>
-      <c r="B11" s="43"/>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="47"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="12">
         <v>3</v>
       </c>
@@ -3093,13 +3455,13 @@
       <c r="F11" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="44" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="45"/>
-      <c r="B12" s="43"/>
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="47"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="12">
         <v>4</v>
       </c>
@@ -3112,32 +3474,32 @@
       <c r="F12" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="G12" s="44" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="44" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="43" t="s">
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="45" t="s">
         <v>156</v>
       </c>
       <c r="C14" s="12">
         <v>2</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="45" t="s">
         <v>172</v>
       </c>
       <c r="E14" s="12">
@@ -3146,46 +3508,46 @@
       <c r="F14" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="44" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="43"/>
-      <c r="B15" s="43"/>
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="45"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="12">
         <v>3</v>
       </c>
-      <c r="D15" s="43"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="12">
         <v>3</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="44" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="43"/>
-      <c r="B16" s="43"/>
+    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="45"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="12">
         <v>4</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="44" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="43" t="s">
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="45" t="s">
         <v>176</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -3203,12 +3565,12 @@
       <c r="F17" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G17" s="52" t="s">
+      <c r="G17" s="44" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="43"/>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="45"/>
       <c r="B18" s="12" t="s">
         <v>161</v>
       </c>
@@ -3224,12 +3586,12 @@
       <c r="F18" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="44" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="43"/>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
       <c r="B19" s="12" t="s">
         <v>161</v>
       </c>
@@ -3245,12 +3607,12 @@
       <c r="F19" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="44" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="43"/>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="45"/>
       <c r="B20" s="12" t="s">
         <v>161</v>
       </c>
@@ -3266,12 +3628,12 @@
       <c r="F20" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G20" s="52" t="s">
+      <c r="G20" s="44" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="43"/>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="45"/>
       <c r="B21" s="12" t="s">
         <v>161</v>
       </c>
@@ -3287,21 +3649,21 @@
       <c r="F21" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G21" s="52" t="s">
+      <c r="G21" s="44" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>184</v>
       </c>
@@ -3321,7 +3683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549BE2A6-D3E1-48AC-89F6-F4291F305CA4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -3329,19 +3691,19 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -3367,7 +3729,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="146.25" customHeight="1">
+    <row r="2" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>193</v>
       </c>
@@ -3384,7 +3746,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>193</v>
       </c>
@@ -3401,7 +3763,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>193</v>
       </c>
@@ -3418,7 +3780,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="195">
+    <row r="5" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>204</v>
       </c>
@@ -3435,7 +3797,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="135">
+    <row r="6" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>204</v>
       </c>
@@ -3457,29 +3819,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6406AA1D-CC82-44BD-A945-6B6CE2716A14}">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="20" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="15.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="20" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="48.5" style="22" customWidth="1"/>
+    <col min="6" max="6" width="37.5" style="22" customWidth="1"/>
+    <col min="7" max="7" width="33.5" style="22" customWidth="1"/>
+    <col min="8" max="8" width="29.5" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="26" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="26" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>211</v>
       </c>
@@ -3502,11 +3864,11 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="105">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A2" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>217</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -3522,9 +3884,9 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49"/>
+    <row r="3" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51"/>
       <c r="D3" s="21" t="s">
         <v>222</v>
       </c>
@@ -3536,9 +3898,9 @@
       </c>
       <c r="G3" s="39"/>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" ht="45">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
+    <row r="4" spans="1:7" s="26" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="49"/>
+      <c r="B4" s="52"/>
       <c r="D4" s="27" t="s">
         <v>225</v>
       </c>
@@ -3552,8 +3914,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="49"/>
       <c r="B5" s="41" t="s">
         <v>229</v>
       </c>
@@ -3569,9 +3931,9 @@
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
     </row>
-    <row r="6" spans="1:7" s="29" customFormat="1" ht="45">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49" t="s">
+    <row r="6" spans="1:7" s="29" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="49"/>
+      <c r="B6" s="51" t="s">
         <v>233</v>
       </c>
       <c r="D6" s="30" t="s">
@@ -3585,9 +3947,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+      <c r="B7" s="51"/>
       <c r="D7" s="21" t="s">
         <v>237</v>
       </c>
@@ -3599,9 +3961,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="47"/>
-      <c r="B8" s="49"/>
+    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="49"/>
+      <c r="B8" s="51"/>
       <c r="D8" s="21" t="s">
         <v>239</v>
       </c>
@@ -3613,9 +3975,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45">
-      <c r="A9" s="47"/>
-      <c r="B9" s="49"/>
+    <row r="9" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+      <c r="B9" s="51"/>
       <c r="D9" s="21" t="s">
         <v>242</v>
       </c>
@@ -3627,9 +3989,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="47"/>
-      <c r="B10" s="49"/>
+    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="49"/>
+      <c r="B10" s="51"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -3643,9 +4005,9 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
+    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="49"/>
+      <c r="B11" s="51"/>
       <c r="D11" s="21" t="s">
         <v>248</v>
       </c>
@@ -3655,9 +4017,9 @@
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
     </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="47"/>
-      <c r="B12" s="49"/>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="49"/>
+      <c r="B12" s="51"/>
       <c r="D12" s="21" t="s">
         <v>16</v>
       </c>
@@ -3667,9 +4029,9 @@
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
     </row>
-    <row r="13" spans="1:7" s="26" customFormat="1" ht="90">
-      <c r="A13" s="47"/>
-      <c r="B13" s="50"/>
+    <row r="13" spans="1:7" s="26" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A13" s="49"/>
+      <c r="B13" s="52"/>
       <c r="D13" s="27" t="s">
         <v>251</v>
       </c>
@@ -3683,9 +4045,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49" t="s">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="49"/>
+      <c r="B14" s="51" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="20" t="s">
@@ -3700,9 +4062,9 @@
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
     </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="49"/>
+      <c r="B15" s="51"/>
       <c r="D15" s="21" t="s">
         <v>258</v>
       </c>
@@ -3712,9 +4074,9 @@
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
     </row>
-    <row r="16" spans="1:7" s="26" customFormat="1" ht="30">
-      <c r="A16" s="47"/>
-      <c r="B16" s="50"/>
+    <row r="16" spans="1:7" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="49"/>
+      <c r="B16" s="52"/>
       <c r="D16" s="27" t="s">
         <v>260</v>
       </c>
@@ -3726,9 +4088,9 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45">
-      <c r="A17" s="47"/>
-      <c r="B17" s="49" t="s">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="49"/>
+      <c r="B17" s="51" t="s">
         <v>263</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -3745,9 +4107,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30">
-      <c r="A18" s="47"/>
-      <c r="B18" s="49"/>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="49"/>
+      <c r="B18" s="51"/>
       <c r="D18" s="21" t="s">
         <v>268</v>
       </c>
@@ -3757,9 +4119,9 @@
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
     </row>
-    <row r="19" spans="1:8" ht="45">
-      <c r="A19" s="47"/>
-      <c r="B19" s="49"/>
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="49"/>
+      <c r="B19" s="51"/>
       <c r="D19" s="21" t="s">
         <v>270</v>
       </c>
@@ -3771,9 +4133,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
+    <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="51"/>
       <c r="D20" s="21" t="s">
         <v>273</v>
       </c>
@@ -3785,9 +4147,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49"/>
+    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="51"/>
       <c r="D21" s="21" t="s">
         <v>276</v>
       </c>
@@ -3799,9 +4161,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="26" customFormat="1" ht="30">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+    <row r="22" spans="1:8" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="49"/>
+      <c r="B22" s="52"/>
       <c r="D22" s="27" t="s">
         <v>278</v>
       </c>
@@ -3813,9 +4175,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="47"/>
-      <c r="B23" s="49" t="s">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="51" t="s">
         <v>281</v>
       </c>
       <c r="D23" s="21" t="s">
@@ -3827,9 +4189,9 @@
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
     </row>
-    <row r="24" spans="1:8" s="26" customFormat="1" ht="30">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+    <row r="24" spans="1:8" s="26" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="52"/>
       <c r="D24" s="27" t="s">
         <v>284</v>
       </c>
@@ -3841,9 +4203,9 @@
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="47"/>
-      <c r="B25" s="49" t="s">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="49"/>
+      <c r="B25" s="51" t="s">
         <v>287</v>
       </c>
       <c r="D25" s="21" t="s">
@@ -3857,9 +4219,9 @@
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30">
-      <c r="A26" s="47"/>
-      <c r="B26" s="49"/>
+    <row r="26" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="49"/>
+      <c r="B26" s="51"/>
       <c r="D26" s="21" t="s">
         <v>291</v>
       </c>
@@ -3871,9 +4233,9 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30">
-      <c r="A27" s="47"/>
-      <c r="B27" s="49"/>
+    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="49"/>
+      <c r="B27" s="51"/>
       <c r="D27" s="21" t="s">
         <v>294</v>
       </c>
@@ -3885,9 +4247,9 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="47"/>
-      <c r="B28" s="49" t="s">
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="49"/>
+      <c r="B28" s="51" t="s">
         <v>297</v>
       </c>
       <c r="C28" s="20" t="s">
@@ -3902,9 +4264,9 @@
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="47"/>
-      <c r="B29" s="49"/>
+    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="49"/>
+      <c r="B29" s="51"/>
       <c r="D29" s="21" t="s">
         <v>301</v>
       </c>
@@ -3915,9 +4277,9 @@
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
     </row>
-    <row r="30" spans="1:8" ht="30">
-      <c r="A30" s="47"/>
-      <c r="B30" s="49"/>
+    <row r="30" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="49"/>
+      <c r="B30" s="51"/>
       <c r="D30" s="21" t="s">
         <v>303</v>
       </c>
@@ -3929,9 +4291,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30">
-      <c r="A31" s="47"/>
-      <c r="B31" s="49"/>
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="49"/>
+      <c r="B31" s="51"/>
       <c r="D31" s="21" t="s">
         <v>145</v>
       </c>
@@ -3943,9 +4305,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30">
-      <c r="A32" s="47"/>
-      <c r="B32" s="49"/>
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="49"/>
+      <c r="B32" s="51"/>
       <c r="D32" s="21" t="s">
         <v>141</v>
       </c>
@@ -3957,9 +4319,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30">
-      <c r="A33" s="47"/>
-      <c r="B33" s="49"/>
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="49"/>
+      <c r="B33" s="51"/>
       <c r="D33" s="21" t="s">
         <v>308</v>
       </c>
@@ -3971,9 +4333,9 @@
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="26" customFormat="1">
-      <c r="A34" s="48"/>
-      <c r="B34" s="50"/>
+    <row r="34" spans="1:7" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="50"/>
+      <c r="B34" s="52"/>
       <c r="D34" s="27" t="s">
         <v>311</v>
       </c>
@@ -4002,12 +4364,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <SharedWithUsers xmlns="6eecfdd9-8b5b-4114-ac92-3a0f32fb9b0a">
+      <UserInfo>
+        <DisplayName>Deni Chen</DisplayName>
+        <AccountId>6</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kate Boxer</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Zarni Htet</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4222,37 +4599,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <SharedWithUsers xmlns="6eecfdd9-8b5b-4114-ac92-3a0f32fb9b0a">
-      <UserInfo>
-        <DisplayName>Deni Chen</DisplayName>
-        <AccountId>6</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kate Boxer</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Zarni Htet</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2398D517-2951-4E1E-AE18-DAD49A3E4730}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF76162-8E32-48E7-8178-54CFC1CA65DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6eecfdd9-8b5b-4114-ac92-3a0f32fb9b0a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2B33AEE-3231-410A-B44F-46603C253084}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2B33AEE-3231-410A-B44F-46603C253084}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a8a7ac9a-5a1e-4647-af62-cc0a29d7a8c3"/>
+    <ds:schemaRef ds:uri="6eecfdd9-8b5b-4114-ac92-3a0f32fb9b0a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF76162-8E32-48E7-8178-54CFC1CA65DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2398D517-2951-4E1E-AE18-DAD49A3E4730}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>